<commit_message>
Looking at hits/FAs across confidence levels in open datasets
</commit_message>
<xml_diff>
--- a/Dataset testing and reports/Power Calculators.xlsx
+++ b/Dataset testing and reports/Power Calculators.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Desktop\poweROC\Dataset testing and reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E040B5F-93CB-4419-9735-C45286A4A7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D827C93-895F-48B9-B25F-C4DB9FBF40DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{1C0BAAFF-5447-44E7-98B6-D28FB95BB2C2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{48CFD621-5A71-3F44-9551-66CA0E00FD5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="pAUC modification" sheetId="3" r:id="rId2"/>
+    <sheet name="Colloff algorithm attempt 1" sheetId="4" r:id="rId3"/>
+    <sheet name="Colloff algorithm attempt 2)" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,19 +37,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Lineup pAUC</t>
-  </si>
-  <si>
-    <t>Showup pAUC</t>
-  </si>
-  <si>
-    <t>D</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+  <si>
+    <t>Tool for calculating Full ROC Sample size</t>
+  </si>
+  <si>
+    <t>True Pos rate</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>Goal N per condition</t>
+  </si>
+  <si>
+    <t>True neg rate</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
+  <si>
+    <t>False pos rate</t>
+  </si>
+  <si>
+    <t>False neg rate</t>
+  </si>
+  <si>
+    <t>TP + FN</t>
+  </si>
+  <si>
+    <t>Prevalence</t>
+  </si>
+  <si>
+    <t>TN + FP</t>
+  </si>
+  <si>
+    <t>Culprit IDs</t>
+  </si>
+  <si>
+    <t>Suspect IDs</t>
+  </si>
+  <si>
+    <t>Correct Rejections</t>
+  </si>
+  <si>
+    <t>CP Total</t>
+  </si>
+  <si>
+    <t>CA Total</t>
+  </si>
+  <si>
+    <t>Grand total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>False Rejections</t>
+  </si>
+  <si>
+    <t>CP Filler selections</t>
+  </si>
+  <si>
+    <t>CA Filler selections</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Lineup </t>
+      <t xml:space="preserve">Buderer, N. M. (1996). Statistical methodology: I. Incorporating the prevalence of disease into the sample size calculation for sensitivity and specificity. </t>
     </r>
     <r>
       <rPr>
@@ -56,12 +116,27 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>N</t>
+      <t>Academy of Emergency Medicine, 3</t>
     </r>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">Showup </t>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(9), 895-900.</t>
+    </r>
+  </si>
+  <si>
+    <t>Negida, A., Fahim, N. K., &amp; Negida, Y. (2019). Sample size calculation guide - part 4: How to </t>
+  </si>
+  <si>
+    <t>calculate the sample size for a diagnostic test accuracy study based on sensitivity, </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">specificity, and the area under the ROC curve. </t>
     </r>
     <r>
       <rPr>
@@ -71,44 +146,104 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>N</t>
+      <t>Advanced Journal of Emergency Medicine, </t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Total </t>
+      <t>3</t>
     </r>
     <r>
       <rPr>
-        <i/>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>N</t>
+      <t>(3), e33. https://doi.org/10.22114/ajem.v0i0.158</t>
     </r>
   </si>
   <si>
-    <t>SE</t>
-  </si>
-  <si>
-    <t>SD</t>
+    <t>Sources:</t>
+  </si>
+  <si>
+    <t>Baratlook A., Hosseini, M., Negida, A., &amp; El Ashal, G. (2015). Part 1: Simple definition and calculation of accuracy, sensitivity, and specificity. Emergency (Tehran), 3(2), 48-49.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Instructions:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Add your data to the "Count" column as raw # of decisions made (B6 to B11), rest will calculate</t>
+    </r>
+  </si>
+  <si>
+    <t>pAUC1</t>
+  </si>
+  <si>
+    <t>pAUC2</t>
+  </si>
+  <si>
+    <t>n1</t>
+  </si>
+  <si>
+    <t>n2</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>sd</t>
   </si>
   <si>
     <t>AUC diff</t>
   </si>
   <si>
-    <t>s (D)</t>
+    <t>Total N</t>
+  </si>
+  <si>
+    <t>Top term</t>
+  </si>
+  <si>
+    <t>Bottom term</t>
+  </si>
+  <si>
+    <t>Power calculator:</t>
+  </si>
+  <si>
+    <t>https://www.sphanalytics.com/statistical-power-calculator-using-average-values/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -126,6 +261,31 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -160,22 +320,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -487,111 +652,628 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{415F871D-709D-47A9-802E-9C57657B4CA4}">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072D3662-B7B0-3F46-A15F-45850E1A56C5}">
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D6">
+        <f>B6/B12</f>
+        <v>0.60869565217391308</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <f>D6/(D6+D9)</f>
+        <v>0.68292682926829273</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <f>B11/B13</f>
+        <v>0.63461538461538458</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <f>D7/(D7+D8)</f>
+        <v>0.63461538461538458</v>
+      </c>
+      <c r="I7">
+        <f>(G9/D10)+(G10/(1-D10))</f>
+        <v>241.6126232411786</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f>(B9+B10)/B13</f>
+        <v>0.36538461538461536</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <f>B7/B12</f>
+        <v>0.28260869565217389</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="G9">
+        <f>(1.64^2)*(G6*(1-G6)/(0.1^2))</f>
+        <v>58.239999999999974</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="1">
-        <v>0.31</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.17</v>
-      </c>
-      <c r="C2" s="1">
-        <f>ABS(A2-B2)</f>
-        <v>0.13999999999999999</v>
-      </c>
-      <c r="D2" s="1">
-        <v>6.13</v>
-      </c>
-      <c r="E2" s="1">
-        <f>C2/D2</f>
-        <v>2.2838499184339313E-2</v>
-      </c>
-      <c r="F2" s="1">
-        <v>424</v>
-      </c>
-      <c r="G2" s="1">
-        <v>455</v>
-      </c>
-      <c r="H2" s="1">
-        <v>879</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="1">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="C3" s="1">
-        <f>ABS(A3-B3)</f>
-        <v>0.12999999999999998</v>
-      </c>
-      <c r="D3" s="1">
-        <v>5.84</v>
-      </c>
-      <c r="E3" s="1">
-        <f>C3/D3</f>
-        <v>2.2260273972602735E-2</v>
-      </c>
-      <c r="F3" s="1">
-        <v>836</v>
-      </c>
-      <c r="G3" s="1">
-        <v>455</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="D10">
+        <f>B12/B14</f>
+        <v>0.46938775510204084</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <f>(1.64^2)*(G7*(1-G7)/(0.1^2))</f>
+        <v>62.366094674556194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <f>B6+B7+B8</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <f>B9+B10+B11</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <f>B12+B13</f>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7FFC27-D961-4259-9840-BCC179B75DE9}">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f>B6/B12</f>
+        <v>0.60869565217391308</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <f>D6/(D6+D9)</f>
+        <v>0.68292682926829273</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <f>B11/B13</f>
+        <v>0.63461538461538458</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <f>D7/(D7+D8)</f>
+        <v>0.63461538461538458</v>
+      </c>
+      <c r="I7">
+        <f>(G9/D10)+(G10/(1-D10))</f>
+        <v>241.6126232411786</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f>(B9+B10)/B13</f>
+        <v>0.36538461538461536</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <f>B7/B12</f>
+        <v>0.28260869565217389</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <f>(1.64^2)*(G6*(1-G6)/(0.1^2))</f>
+        <v>58.239999999999974</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <f>B12/B14</f>
+        <v>0.46938775510204084</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <f>(1.64^2)*(G7*(1-G7)/(0.1^2))</f>
+        <v>62.366094674556194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <f>B6+B7+B8</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <f>B9+B10+B11</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <f>B12+B13</f>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C9C2AEE-4269-4DFF-BFFC-9DE110150B68}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="C2" s="6">
+        <f>ABS(A2-B2)</f>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="D2" s="6">
+        <v>424</v>
+      </c>
+      <c r="E2" s="6">
+        <v>455</v>
+      </c>
+      <c r="F2" s="6">
+        <f>D2+E2</f>
+        <v>879</v>
+      </c>
+      <c r="G2" s="6">
+        <v>6.13</v>
+      </c>
+      <c r="H2">
+        <f>C2/G2</f>
+        <v>2.2838499184339313E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H4" r:id="rId1" xr:uid="{9687370E-52A7-4E58-B548-98B53C6C50F7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B6254A-7946-4145-A45B-13E5E89138E1}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="C2" s="6">
+        <f>ABS(A2-B2)</f>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="D2" s="6">
+        <v>424</v>
+      </c>
+      <c r="E2" s="6">
+        <v>455</v>
+      </c>
+      <c r="F2" s="6">
+        <f>D2+E2</f>
+        <v>879</v>
+      </c>
+      <c r="G2" s="6">
+        <v>6.13</v>
+      </c>
+      <c r="H2" s="7">
+        <f>(E2*(A2^2)*D2) - (2*E2*A2*B2*D2) + (E2*(B2^2)*D2)</f>
+        <v>3781.2319999999991</v>
+      </c>
+      <c r="I2" s="7">
+        <f>(G2^2)*(D2+E2)</f>
+        <v>33030.095099999999</v>
+      </c>
+      <c r="J2">
+        <f>SQRT(H2/I2)</f>
+        <v>0.33834654824934168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J4" r:id="rId1" xr:uid="{4E304558-F2A5-4F0F-B703-06E39BD957BD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>